<commit_message>
right now everything works
</commit_message>
<xml_diff>
--- a/FDA_Drug_Trials_Snapshots_2015-19 - US vs ex-US.xlsx
+++ b/FDA_Drug_Trials_Snapshots_2015-19 - US vs ex-US.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcarmeli/Documents/GitHub/FDA_DTS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275BE346-7B1B-CE45-B07D-4E79E74C3A5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0E2D15-ABF5-D241-B65F-59B18E630E5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{2397A3E8-F889-6E44-8C19-9398011308FF}"/>
   </bookViews>
@@ -1948,10 +1948,10 @@
   <dimension ref="A1:AA237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A41" sqref="A41"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>